<commit_message>
Combinations with grid number
</commit_message>
<xml_diff>
--- a/ComponentOptionsTable.xlsx
+++ b/ComponentOptionsTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egh\Source\Egil.RazorComponents.Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8984D4-8374-425A-B5B7-AE30D7C6FCB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BEAA6F-7001-4EB1-A5FC-37E41B0B50A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{013C2776-BE27-4B4D-A298-EF6AEA85CDDD}"/>
   </bookViews>
@@ -68,15 +68,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>Breakpoint</t>
   </si>
   <si>
-    <t>BreakpointNumber</t>
-  </si>
-  <si>
     <t>Auto</t>
   </si>
   <si>
@@ -213,13 +207,19 @@
   </si>
   <si>
     <t>offset</t>
+  </si>
+  <si>
+    <t>GridNumber</t>
+  </si>
+  <si>
+    <t>GridBreakpoint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,12 +256,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -360,7 +354,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -371,7 +365,7 @@
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF92D050"/>
@@ -389,16 +383,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -738,7 +722,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,262 +734,262 @@
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="12" t="s">
-        <v>37</v>
-      </c>
       <c r="K3" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1075,69 +1059,69 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alignment options and parameters
</commit_message>
<xml_diff>
--- a/ComponentOptionsTable.xlsx
+++ b/ComponentOptionsTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egh\Source\Egil.RazorComponents.Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BEAA6F-7001-4EB1-A5FC-37E41B0B50A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDA2A06-B40B-4C99-A900-B98C0BB18F0F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{013C2776-BE27-4B4D-A298-EF6AEA85CDDD}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
   <si>
     <t>Breakpoint</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>GridBreakpoint</t>
+  </si>
+  <si>
+    <t>Container</t>
   </si>
 </sst>
 </file>
@@ -722,7 +725,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +758,7 @@
         <v>25</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
New client test projects, better css class aggregation for compoments
</commit_message>
<xml_diff>
--- a/ComponentOptionsTable.xlsx
+++ b/ComponentOptionsTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egh\Source\Egil.RazorComponents.Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDA2A06-B40B-4C99-A900-B98C0BB18F0F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80915BC5-1BD0-44F2-8C1F-B188939734AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{013C2776-BE27-4B4D-A298-EF6AEA85CDDD}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Col params'!$A$1:$K$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -725,13 +726,15 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="15" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="1" customWidth="1"/>
+    <col min="8" max="15" width="12.7109375" style="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>

</xml_diff>